<commit_message>
1.update the kellyb for kgoodlist
</commit_message>
<xml_diff>
--- a/braised.xlsx
+++ b/braised.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>code</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>expval</t>
+  </si>
+  <si>
+    <t>lastyear</t>
   </si>
   <si>
     <t>sh113570</t>
@@ -1109,7 +1112,7 @@
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D15"/>
+      <selection activeCell="A2" sqref="A2:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1133,7 +1136,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1142,10 +1147,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
         <v>2.798</v>
@@ -1153,14 +1158,16 @@
       <c r="D2" s="2">
         <v>114.214925892533</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="2">
+        <v>3.214</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2">
         <v>2.972</v>
@@ -1168,14 +1175,16 @@
       <c r="D3" s="2">
         <v>107.349135486632</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="2">
+        <v>1.011</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2">
         <v>3.099</v>
@@ -1183,14 +1192,16 @@
       <c r="D4" s="2">
         <v>114.23402617933</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="2">
+        <v>3.014</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2">
         <v>2.249</v>
@@ -1198,14 +1209,16 @@
       <c r="D5" s="2">
         <v>116.975795817404</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="2">
+        <v>3.178</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2">
         <v>3.631</v>
@@ -1213,14 +1226,16 @@
       <c r="D6" s="2">
         <v>112.016445935932</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="2">
+        <v>1.932</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2">
         <v>3.372</v>
@@ -1228,14 +1243,16 @@
       <c r="D7" s="2">
         <v>123.047092024649</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="2">
+        <v>2.984</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2">
         <v>2.137</v>
@@ -1243,14 +1260,16 @@
       <c r="D8" s="2">
         <v>113.261680808724</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="2">
+        <v>2.811</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2">
         <v>2.945</v>
@@ -1258,14 +1277,16 @@
       <c r="D9" s="2">
         <v>115.280357396625</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2">
         <v>2.171</v>
@@ -1273,14 +1294,16 @@
       <c r="D10" s="2">
         <v>116.80738868174</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="2">
+        <v>3.304</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2">
         <v>2.999</v>
@@ -1288,14 +1311,16 @@
       <c r="D11" s="2">
         <v>113.365144533126</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="2">
+        <v>2.647</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2">
         <v>2.297</v>
@@ -1303,14 +1328,16 @@
       <c r="D12" s="2">
         <v>118.630076524064</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="2">
+        <v>2.833</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2">
         <v>3.297</v>
@@ -1318,14 +1345,16 @@
       <c r="D13" s="2">
         <v>114.793358892158</v>
       </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="2">
+        <v>1.978</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2">
         <v>1.499</v>
@@ -1333,13 +1362,16 @@
       <c r="D14" s="2">
         <v>117.163217039191</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="2">
+        <v>3.022</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" s="2">
         <v>3.746</v>
@@ -1347,78 +1379,81 @@
       <c r="D15" s="2">
         <v>123.180565334798</v>
       </c>
+      <c r="E15" s="2">
+        <v>3.307</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3"/>

</xml_diff>

<commit_message>
1.give the difference between policy 1 and policy 2
</commit_message>
<xml_diff>
--- a/braised.xlsx
+++ b/braised.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7270"/>
+    <workbookView windowWidth="18530" windowHeight="6670"/>
   </bookViews>
   <sheets>
     <sheet name="clause" sheetId="2" r:id="rId1"/>
@@ -31,16 +31,16 @@
     <t>lastyear</t>
   </si>
   <si>
-    <t>sh113570</t>
-  </si>
-  <si>
-    <t>百达转债</t>
-  </si>
-  <si>
-    <t>sz128033</t>
-  </si>
-  <si>
-    <t>迪龙转债</t>
+    <t>sz128042</t>
+  </si>
+  <si>
+    <t>凯中转债</t>
+  </si>
+  <si>
+    <t>sz128076</t>
+  </si>
+  <si>
+    <t>金轮转债</t>
   </si>
   <si>
     <t>sz128090</t>
@@ -55,34 +55,52 @@
     <t>宏辉转债</t>
   </si>
   <si>
+    <t>sz128085</t>
+  </si>
+  <si>
+    <t>鸿达转债</t>
+  </si>
+  <si>
+    <t>sh113532</t>
+  </si>
+  <si>
+    <t>海环转债</t>
+  </si>
+  <si>
+    <t>sh110070</t>
+  </si>
+  <si>
+    <t>凌钢转债</t>
+  </si>
+  <si>
+    <t>sz128066</t>
+  </si>
+  <si>
+    <t>亚泰转债</t>
+  </si>
+  <si>
+    <t>sh113030</t>
+  </si>
+  <si>
+    <t>东风转债</t>
+  </si>
+  <si>
     <t>sz128049</t>
   </si>
   <si>
     <t>华源转债</t>
   </si>
   <si>
-    <t>sz128085</t>
-  </si>
-  <si>
-    <t>鸿达转债</t>
-  </si>
-  <si>
-    <t>sz128076</t>
-  </si>
-  <si>
-    <t>金轮转债</t>
-  </si>
-  <si>
-    <t>sh113030</t>
-  </si>
-  <si>
-    <t>东风转债</t>
-  </si>
-  <si>
-    <t>sh110070</t>
-  </si>
-  <si>
-    <t>凌钢转债</t>
+    <t>sh113546</t>
+  </si>
+  <si>
+    <t>迪贝转债</t>
+  </si>
+  <si>
+    <t>sz123010</t>
+  </si>
+  <si>
+    <t>博世转债</t>
   </si>
   <si>
     <t>sz128071</t>
@@ -91,28 +109,10 @@
     <t>合兴转债</t>
   </si>
   <si>
-    <t>sh113546</t>
-  </si>
-  <si>
-    <t>迪贝转债</t>
-  </si>
-  <si>
     <t>sh113524</t>
   </si>
   <si>
     <t>奇精转债</t>
-  </si>
-  <si>
-    <t>sh113561</t>
-  </si>
-  <si>
-    <t>正裕转债</t>
-  </si>
-  <si>
-    <t>sz123050</t>
-  </si>
-  <si>
-    <t>聚飞转债</t>
   </si>
 </sst>
 </file>
@@ -1153,13 +1153,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>2.798</v>
+        <v>4.154</v>
       </c>
       <c r="D2" s="2">
-        <v>114.214925892533</v>
+        <v>113.756915790339</v>
       </c>
       <c r="E2" s="2">
-        <v>3.214</v>
+        <v>1.589</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1170,13 +1170,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="2">
-        <v>2.972</v>
+        <v>2.137</v>
       </c>
       <c r="D3" s="2">
-        <v>107.349135486632</v>
+        <v>113.213232270377</v>
       </c>
       <c r="E3" s="2">
-        <v>1.011</v>
+        <v>2.797</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1190,10 +1190,10 @@
         <v>3.099</v>
       </c>
       <c r="D4" s="2">
-        <v>114.23402617933</v>
+        <v>113.223424639238</v>
       </c>
       <c r="E4" s="2">
-        <v>3.014</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1207,10 +1207,10 @@
         <v>2.249</v>
       </c>
       <c r="D5" s="2">
-        <v>116.975795817404</v>
+        <v>116.979893295546</v>
       </c>
       <c r="E5" s="2">
-        <v>3.178</v>
+        <v>3.164</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1221,13 +1221,13 @@
         <v>14</v>
       </c>
       <c r="C6" s="2">
-        <v>3.631</v>
+        <v>3.372</v>
       </c>
       <c r="D6" s="2">
-        <v>112.016445935932</v>
+        <v>123.047304851407</v>
       </c>
       <c r="E6" s="2">
-        <v>1.932</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1238,13 +1238,13 @@
         <v>16</v>
       </c>
       <c r="C7" s="2">
-        <v>3.372</v>
+        <v>4.585</v>
       </c>
       <c r="D7" s="2">
-        <v>123.047092024649</v>
+        <v>111.296374183947</v>
       </c>
       <c r="E7" s="2">
-        <v>2.984</v>
+        <v>2.26</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1255,13 +1255,13 @@
         <v>18</v>
       </c>
       <c r="C8" s="2">
-        <v>2.137</v>
+        <v>2.171</v>
       </c>
       <c r="D8" s="2">
-        <v>113.261680808724</v>
+        <v>116.79640553509</v>
       </c>
       <c r="E8" s="2">
-        <v>2.811</v>
+        <v>3.29</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1272,13 +1272,13 @@
         <v>20</v>
       </c>
       <c r="C9" s="2">
-        <v>2.945</v>
+        <v>4.61</v>
       </c>
       <c r="D9" s="2">
-        <v>115.280357396625</v>
+        <v>115.550058680819</v>
       </c>
       <c r="E9" s="2">
-        <v>3</v>
+        <v>2.304</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1289,13 +1289,13 @@
         <v>22</v>
       </c>
       <c r="C10" s="2">
-        <v>2.171</v>
+        <v>2.945</v>
       </c>
       <c r="D10" s="2">
-        <v>116.80738868174</v>
+        <v>115.258763828604</v>
       </c>
       <c r="E10" s="2">
-        <v>3.304</v>
+        <v>2.989</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1306,13 +1306,13 @@
         <v>24</v>
       </c>
       <c r="C11" s="2">
-        <v>2.999</v>
+        <v>3.631</v>
       </c>
       <c r="D11" s="2">
-        <v>113.365144533126</v>
+        <v>112.004522833776</v>
       </c>
       <c r="E11" s="2">
-        <v>2.647</v>
+        <v>1.918</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1326,10 +1326,10 @@
         <v>2.297</v>
       </c>
       <c r="D12" s="2">
-        <v>118.630076524064</v>
+        <v>118.624606427396</v>
       </c>
       <c r="E12" s="2">
-        <v>2.833</v>
+        <v>2.819</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1340,13 +1340,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="2">
-        <v>3.297</v>
+        <v>4.296</v>
       </c>
       <c r="D13" s="2">
-        <v>114.793358892158</v>
+        <v>109.796697972964</v>
       </c>
       <c r="E13" s="2">
-        <v>1.978</v>
+        <v>1.521</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1357,13 +1357,13 @@
         <v>30</v>
       </c>
       <c r="C14" s="2">
-        <v>1.499</v>
+        <v>2.999</v>
       </c>
       <c r="D14" s="2">
-        <v>117.163217039191</v>
+        <v>113.3441879442</v>
       </c>
       <c r="E14" s="2">
-        <v>3.022</v>
+        <v>2.633</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1374,13 +1374,13 @@
         <v>32</v>
       </c>
       <c r="C15" s="2">
-        <v>3.746</v>
+        <v>3.297</v>
       </c>
       <c r="D15" s="2">
-        <v>123.180565334798</v>
+        <v>114.792334273914</v>
       </c>
       <c r="E15" s="2">
-        <v>3.307</v>
+        <v>1.964</v>
       </c>
     </row>
     <row r="16" spans="1:4">

</xml_diff>

<commit_message>
BIG BIG FIXED 1.bombs winrate computed by bond premium rate 2.missile winrate computed by distance
</commit_message>
<xml_diff>
--- a/braised.xlsx
+++ b/braised.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="6670"/>
+    <workbookView windowWidth="18530" windowHeight="7270"/>
   </bookViews>
   <sheets>
     <sheet name="clause" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>code</t>
   </si>
@@ -31,10 +31,34 @@
     <t>lastyear</t>
   </si>
   <si>
-    <t>sz128042</t>
-  </si>
-  <si>
-    <t>凯中转债</t>
+    <t>sh113591</t>
+  </si>
+  <si>
+    <t>胜达转债</t>
+  </si>
+  <si>
+    <t>sh113595</t>
+  </si>
+  <si>
+    <t>花王转债</t>
+  </si>
+  <si>
+    <t>sz128097</t>
+  </si>
+  <si>
+    <t>奥佳转债</t>
+  </si>
+  <si>
+    <t>sz128090</t>
+  </si>
+  <si>
+    <t>汽模转2</t>
+  </si>
+  <si>
+    <t>sh113565</t>
+  </si>
+  <si>
+    <t>宏辉转债</t>
   </si>
   <si>
     <t>sz128076</t>
@@ -43,16 +67,10 @@
     <t>金轮转债</t>
   </si>
   <si>
-    <t>sz128090</t>
-  </si>
-  <si>
-    <t>汽模转2</t>
-  </si>
-  <si>
-    <t>sh113565</t>
-  </si>
-  <si>
-    <t>宏辉转债</t>
+    <t>sh113532</t>
+  </si>
+  <si>
+    <t>海环转债</t>
   </si>
   <si>
     <t>sz128085</t>
@@ -61,10 +79,10 @@
     <t>鸿达转债</t>
   </si>
   <si>
-    <t>sh113532</t>
-  </si>
-  <si>
-    <t>海环转债</t>
+    <t>sz128066</t>
+  </si>
+  <si>
+    <t>亚泰转债</t>
   </si>
   <si>
     <t>sh110070</t>
@@ -73,22 +91,16 @@
     <t>凌钢转债</t>
   </si>
   <si>
-    <t>sz128066</t>
-  </si>
-  <si>
-    <t>亚泰转债</t>
-  </si>
-  <si>
     <t>sh113030</t>
   </si>
   <si>
     <t>东风转债</t>
   </si>
   <si>
-    <t>sz128049</t>
-  </si>
-  <si>
-    <t>华源转债</t>
+    <t>sz128071</t>
+  </si>
+  <si>
+    <t>合兴转债</t>
   </si>
   <si>
     <t>sh113546</t>
@@ -97,22 +109,28 @@
     <t>迪贝转债</t>
   </si>
   <si>
-    <t>sz123010</t>
-  </si>
-  <si>
-    <t>博世转债</t>
-  </si>
-  <si>
-    <t>sz128071</t>
-  </si>
-  <si>
-    <t>合兴转债</t>
-  </si>
-  <si>
-    <t>sh113524</t>
-  </si>
-  <si>
-    <t>奇精转债</t>
+    <t>sz123087</t>
+  </si>
+  <si>
+    <t>明电转债</t>
+  </si>
+  <si>
+    <t>sz123127</t>
+  </si>
+  <si>
+    <t>耐普转债</t>
+  </si>
+  <si>
+    <t>sh113561</t>
+  </si>
+  <si>
+    <t>正裕转债</t>
+  </si>
+  <si>
+    <t>sz123082</t>
+  </si>
+  <si>
+    <t>北陆转债</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1130,7 @@
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E15"/>
+      <selection activeCell="A2" sqref="A2:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1153,13 +1171,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>4.154</v>
+        <v>4.743</v>
       </c>
       <c r="D2" s="2">
-        <v>113.756915790339</v>
+        <v>121.088723742528</v>
       </c>
       <c r="E2" s="2">
-        <v>1.589</v>
+        <v>3.501</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1170,13 +1188,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="2">
-        <v>2.137</v>
+        <v>3.298</v>
       </c>
       <c r="D3" s="2">
-        <v>113.213232270377</v>
+        <v>124.386135388323</v>
       </c>
       <c r="E3" s="2">
-        <v>2.797</v>
+        <v>3.556</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1187,13 +1205,13 @@
         <v>10</v>
       </c>
       <c r="C4" s="2">
-        <v>3.099</v>
+        <v>4.583</v>
       </c>
       <c r="D4" s="2">
-        <v>113.223424639238</v>
+        <v>114.305645541136</v>
       </c>
       <c r="E4" s="2">
-        <v>3</v>
+        <v>3.159</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1204,13 +1222,13 @@
         <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>2.249</v>
+        <v>3.099</v>
       </c>
       <c r="D5" s="2">
-        <v>116.979893295546</v>
+        <v>113.243772082912</v>
       </c>
       <c r="E5" s="2">
-        <v>3.164</v>
+        <v>2.995</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1221,13 +1239,13 @@
         <v>14</v>
       </c>
       <c r="C6" s="2">
-        <v>3.372</v>
+        <v>2.249</v>
       </c>
       <c r="D6" s="2">
-        <v>123.047304851407</v>
+        <v>116.999862356903</v>
       </c>
       <c r="E6" s="2">
-        <v>2.97</v>
+        <v>3.159</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1238,13 +1256,13 @@
         <v>16</v>
       </c>
       <c r="C7" s="2">
-        <v>4.585</v>
+        <v>2.137</v>
       </c>
       <c r="D7" s="2">
-        <v>111.296374183947</v>
+        <v>113.231907120925</v>
       </c>
       <c r="E7" s="2">
-        <v>2.26</v>
+        <v>2.792</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1255,13 +1273,13 @@
         <v>18</v>
       </c>
       <c r="C8" s="2">
-        <v>2.171</v>
+        <v>4.585</v>
       </c>
       <c r="D8" s="2">
-        <v>116.79640553509</v>
+        <v>111.330072713379</v>
       </c>
       <c r="E8" s="2">
-        <v>3.29</v>
+        <v>2.255</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1272,13 +1290,13 @@
         <v>20</v>
       </c>
       <c r="C9" s="2">
-        <v>4.61</v>
+        <v>3.372</v>
       </c>
       <c r="D9" s="2">
-        <v>115.550058680819</v>
+        <v>123.056827834803</v>
       </c>
       <c r="E9" s="2">
-        <v>2.304</v>
+        <v>2.964</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1289,13 +1307,13 @@
         <v>22</v>
       </c>
       <c r="C10" s="2">
-        <v>2.945</v>
+        <v>4.61</v>
       </c>
       <c r="D10" s="2">
-        <v>115.258763828604</v>
+        <v>115.600951185195</v>
       </c>
       <c r="E10" s="2">
-        <v>2.989</v>
+        <v>2.299</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1306,13 +1324,13 @@
         <v>24</v>
       </c>
       <c r="C11" s="2">
-        <v>3.631</v>
+        <v>2.171</v>
       </c>
       <c r="D11" s="2">
-        <v>112.004522833776</v>
+        <v>116.809242990561</v>
       </c>
       <c r="E11" s="2">
-        <v>1.918</v>
+        <v>3.285</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1323,13 +1341,13 @@
         <v>26</v>
       </c>
       <c r="C12" s="2">
-        <v>2.297</v>
+        <v>2.945</v>
       </c>
       <c r="D12" s="2">
-        <v>118.624606427396</v>
+        <v>115.268450034347</v>
       </c>
       <c r="E12" s="2">
-        <v>2.819</v>
+        <v>2.984</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1340,13 +1358,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="2">
-        <v>4.296</v>
+        <v>2.999</v>
       </c>
       <c r="D13" s="2">
-        <v>109.796697972964</v>
+        <v>113.365042963786</v>
       </c>
       <c r="E13" s="2">
-        <v>1.521</v>
+        <v>2.627</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1357,13 +1375,13 @@
         <v>30</v>
       </c>
       <c r="C14" s="2">
-        <v>2.999</v>
+        <v>2.297</v>
       </c>
       <c r="D14" s="2">
-        <v>113.3441879442</v>
+        <v>118.597040134681</v>
       </c>
       <c r="E14" s="2">
-        <v>2.633</v>
+        <v>2.814</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1374,32 +1392,65 @@
         <v>32</v>
       </c>
       <c r="C15" s="2">
-        <v>3.297</v>
+        <v>4.189</v>
       </c>
       <c r="D15" s="2">
-        <v>114.792334273914</v>
+        <v>120.128347245463</v>
       </c>
       <c r="E15" s="2">
-        <v>1.964</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+        <v>3.959</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3.999</v>
+      </c>
+      <c r="D16" s="2">
+        <v>115.893419321157</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4.833</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.499</v>
+      </c>
+      <c r="D17" s="2">
+        <v>115.950871731347</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="2">
+        <v>4.993</v>
+      </c>
+      <c r="D18" s="2">
+        <v>120.764775268163</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3.937</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3"/>

</xml_diff>

<commit_message>
1.combie selected and brasied to selected 2.give them same condition price,lasttime,lastmoney
</commit_message>
<xml_diff>
--- a/braised.xlsx
+++ b/braised.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>code</t>
   </si>
@@ -31,16 +31,304 @@
     <t>lastyear</t>
   </si>
   <si>
+    <t>sh113578</t>
+  </si>
+  <si>
+    <t>全筑转债</t>
+  </si>
+  <si>
+    <t>sz128138</t>
+  </si>
+  <si>
+    <t>侨银转债</t>
+  </si>
+  <si>
+    <t>sz123126</t>
+  </si>
+  <si>
+    <t>瑞丰转债</t>
+  </si>
+  <si>
+    <t>sh113608</t>
+  </si>
+  <si>
+    <t>威派转债</t>
+  </si>
+  <si>
+    <t>sz128125</t>
+  </si>
+  <si>
+    <t>华阳转债</t>
+  </si>
+  <si>
+    <t>sh113624</t>
+  </si>
+  <si>
+    <t>正川转债</t>
+  </si>
+  <si>
+    <t>sz128118</t>
+  </si>
+  <si>
+    <t>瀛通转债</t>
+  </si>
+  <si>
+    <t>sz123106</t>
+  </si>
+  <si>
+    <t>正丹转债</t>
+  </si>
+  <si>
+    <t>sh113628</t>
+  </si>
+  <si>
+    <t>晨丰转债</t>
+  </si>
+  <si>
+    <t>sh113610</t>
+  </si>
+  <si>
+    <t>灵康转债</t>
+  </si>
+  <si>
+    <t>sh113593</t>
+  </si>
+  <si>
+    <t>沪工转债</t>
+  </si>
+  <si>
+    <t>sh113573</t>
+  </si>
+  <si>
+    <t>纵横转债</t>
+  </si>
+  <si>
+    <t>sz123082</t>
+  </si>
+  <si>
+    <t>北陆转债</t>
+  </si>
+  <si>
+    <t>sh113600</t>
+  </si>
+  <si>
+    <t>新星转债</t>
+  </si>
+  <si>
+    <t>sz123093</t>
+  </si>
+  <si>
+    <t>金陵转债</t>
+  </si>
+  <si>
+    <t>sz128072</t>
+  </si>
+  <si>
+    <t>翔鹭转债</t>
+  </si>
+  <si>
+    <t>sz128117</t>
+  </si>
+  <si>
+    <t>道恩转债</t>
+  </si>
+  <si>
+    <t>sh113527</t>
+  </si>
+  <si>
+    <t>维格转债</t>
+  </si>
+  <si>
+    <t>sz123059</t>
+  </si>
+  <si>
+    <t>银信转债</t>
+  </si>
+  <si>
+    <t>sz123116</t>
+  </si>
+  <si>
+    <t>万兴转债</t>
+  </si>
+  <si>
+    <t>sz123050</t>
+  </si>
+  <si>
+    <t>聚飞转债</t>
+  </si>
+  <si>
+    <t>sh113566</t>
+  </si>
+  <si>
+    <t>翔港转债</t>
+  </si>
+  <si>
+    <t>sz123100</t>
+  </si>
+  <si>
+    <t>朗科转债</t>
+  </si>
+  <si>
+    <t>sz123039</t>
+  </si>
+  <si>
+    <t>开润转债</t>
+  </si>
+  <si>
+    <t>sz123109</t>
+  </si>
+  <si>
+    <t>昌红转债</t>
+  </si>
+  <si>
+    <t>sz128123</t>
+  </si>
+  <si>
+    <t>国光转债</t>
+  </si>
+  <si>
+    <t>sz123065</t>
+  </si>
+  <si>
+    <t>宝莱转债</t>
+  </si>
+  <si>
+    <t>sh113594</t>
+  </si>
+  <si>
+    <t>淳中转债</t>
+  </si>
+  <si>
+    <t>sz128066</t>
+  </si>
+  <si>
+    <t>亚泰转债</t>
+  </si>
+  <si>
+    <t>sz123087</t>
+  </si>
+  <si>
+    <t>明电转债</t>
+  </si>
+  <si>
+    <t>sh110070</t>
+  </si>
+  <si>
+    <t>凌钢转债</t>
+  </si>
+  <si>
+    <t>sz123061</t>
+  </si>
+  <si>
+    <t>航新转债</t>
+  </si>
+  <si>
+    <t>sh110058</t>
+  </si>
+  <si>
+    <t>永鼎转债</t>
+  </si>
+  <si>
+    <t>sz128071</t>
+  </si>
+  <si>
+    <t>合兴转债</t>
+  </si>
+  <si>
+    <t>sh113597</t>
+  </si>
+  <si>
+    <t>佳力转债</t>
+  </si>
+  <si>
     <t>sh113591</t>
   </si>
   <si>
     <t>胜达转债</t>
   </si>
   <si>
-    <t>sh113595</t>
-  </si>
-  <si>
-    <t>花王转债</t>
+    <t>sh113574</t>
+  </si>
+  <si>
+    <t>华体转债</t>
+  </si>
+  <si>
+    <t>sz123088</t>
+  </si>
+  <si>
+    <t>威唐转债</t>
+  </si>
+  <si>
+    <t>sz128143</t>
+  </si>
+  <si>
+    <t>锋龙转债</t>
+  </si>
+  <si>
+    <t>sh113532</t>
+  </si>
+  <si>
+    <t>海环转债</t>
+  </si>
+  <si>
+    <t>sz123127</t>
+  </si>
+  <si>
+    <t>耐普转债</t>
+  </si>
+  <si>
+    <t>sz128120</t>
+  </si>
+  <si>
+    <t>联诚转债</t>
+  </si>
+  <si>
+    <t>sh113546</t>
+  </si>
+  <si>
+    <t>迪贝转债</t>
+  </si>
+  <si>
+    <t>sh113565</t>
+  </si>
+  <si>
+    <t>宏辉转债</t>
+  </si>
+  <si>
+    <t>sz123089</t>
+  </si>
+  <si>
+    <t>九洲转2</t>
+  </si>
+  <si>
+    <t>sz123048</t>
+  </si>
+  <si>
+    <t>应急转债</t>
+  </si>
+  <si>
+    <t>sh113030</t>
+  </si>
+  <si>
+    <t>东风转债</t>
+  </si>
+  <si>
+    <t>sz128056</t>
+  </si>
+  <si>
+    <t>今飞转债</t>
+  </si>
+  <si>
+    <t>sh113561</t>
+  </si>
+  <si>
+    <t>正裕转债</t>
+  </si>
+  <si>
+    <t>sz123130</t>
+  </si>
+  <si>
+    <t>设研转债</t>
   </si>
   <si>
     <t>sz128097</t>
@@ -55,10 +343,10 @@
     <t>汽模转2</t>
   </si>
   <si>
-    <t>sh113565</t>
-  </si>
-  <si>
-    <t>宏辉转债</t>
+    <t>sz128070</t>
+  </si>
+  <si>
+    <t>智能转债</t>
   </si>
   <si>
     <t>sz128076</t>
@@ -67,70 +355,22 @@
     <t>金轮转债</t>
   </si>
   <si>
-    <t>sh113532</t>
-  </si>
-  <si>
-    <t>海环转债</t>
-  </si>
-  <si>
-    <t>sz128085</t>
-  </si>
-  <si>
-    <t>鸿达转债</t>
-  </si>
-  <si>
-    <t>sz128066</t>
-  </si>
-  <si>
-    <t>亚泰转债</t>
-  </si>
-  <si>
-    <t>sh110070</t>
-  </si>
-  <si>
-    <t>凌钢转债</t>
-  </si>
-  <si>
-    <t>sh113030</t>
-  </si>
-  <si>
-    <t>东风转债</t>
-  </si>
-  <si>
-    <t>sz128071</t>
-  </si>
-  <si>
-    <t>合兴转债</t>
-  </si>
-  <si>
-    <t>sh113546</t>
-  </si>
-  <si>
-    <t>迪贝转债</t>
-  </si>
-  <si>
-    <t>sz123087</t>
-  </si>
-  <si>
-    <t>明电转债</t>
-  </si>
-  <si>
-    <t>sz123127</t>
-  </si>
-  <si>
-    <t>耐普转债</t>
-  </si>
-  <si>
-    <t>sh113561</t>
-  </si>
-  <si>
-    <t>正裕转债</t>
-  </si>
-  <si>
-    <t>sz123082</t>
-  </si>
-  <si>
-    <t>北陆转债</t>
+    <t>sh113570</t>
+  </si>
+  <si>
+    <t>百达转债</t>
+  </si>
+  <si>
+    <t>sz128122</t>
+  </si>
+  <si>
+    <t>兴森转债</t>
+  </si>
+  <si>
+    <t>sz127021</t>
+  </si>
+  <si>
+    <t>特发转2</t>
   </si>
 </sst>
 </file>
@@ -772,13 +1012,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1129,8 +1368,8 @@
   <sheetPr/>
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1171,13 +1410,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>4.743</v>
+        <v>3.838</v>
       </c>
       <c r="D2" s="2">
-        <v>121.088723742528</v>
+        <v>117.693846392957</v>
       </c>
       <c r="E2" s="2">
-        <v>3.501</v>
+        <v>3.307</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1188,13 +1427,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="2">
-        <v>3.298</v>
+        <v>4.199</v>
       </c>
       <c r="D3" s="2">
-        <v>124.386135388323</v>
+        <v>135.917227708266</v>
       </c>
       <c r="E3" s="2">
-        <v>3.556</v>
+        <v>3.885</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1205,13 +1444,13 @@
         <v>10</v>
       </c>
       <c r="C4" s="2">
-        <v>4.583</v>
+        <v>3.4</v>
       </c>
       <c r="D4" s="2">
-        <v>114.305645541136</v>
+        <v>129.774633937819</v>
       </c>
       <c r="E4" s="2">
-        <v>3.159</v>
+        <v>4.701</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1222,13 +1461,13 @@
         <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>3.099</v>
+        <v>4.2</v>
       </c>
       <c r="D5" s="2">
-        <v>113.243772082912</v>
+        <v>120.758880752657</v>
       </c>
       <c r="E5" s="2">
-        <v>2.995</v>
+        <v>3.863</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1239,13 +1478,13 @@
         <v>14</v>
       </c>
       <c r="C6" s="2">
-        <v>2.249</v>
+        <v>4.498</v>
       </c>
       <c r="D6" s="2">
-        <v>116.999862356903</v>
+        <v>117.759257391535</v>
       </c>
       <c r="E6" s="2">
-        <v>3.159</v>
+        <v>3.584</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1256,13 +1495,13 @@
         <v>16</v>
       </c>
       <c r="C7" s="2">
-        <v>2.137</v>
+        <v>4.049</v>
       </c>
       <c r="D7" s="2">
-        <v>113.231907120925</v>
+        <v>121.530967799202</v>
       </c>
       <c r="E7" s="2">
-        <v>2.792</v>
+        <v>4.329</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1273,13 +1512,13 @@
         <v>18</v>
       </c>
       <c r="C8" s="2">
-        <v>4.585</v>
+        <v>2.996</v>
       </c>
       <c r="D8" s="2">
-        <v>111.330072713379</v>
+        <v>121.307979568007</v>
       </c>
       <c r="E8" s="2">
-        <v>2.255</v>
+        <v>3.507</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1290,13 +1529,13 @@
         <v>20</v>
       </c>
       <c r="C9" s="2">
-        <v>3.372</v>
+        <v>3.2</v>
       </c>
       <c r="D9" s="2">
-        <v>123.056827834803</v>
+        <v>125.403965734134</v>
       </c>
       <c r="E9" s="2">
-        <v>2.964</v>
+        <v>4.233</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1307,13 +1546,13 @@
         <v>22</v>
       </c>
       <c r="C10" s="2">
-        <v>4.61</v>
+        <v>4.15</v>
       </c>
       <c r="D10" s="2">
-        <v>115.600951185195</v>
+        <v>121.543055151578</v>
       </c>
       <c r="E10" s="2">
-        <v>2.299</v>
+        <v>4.652</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1324,13 +1563,13 @@
         <v>24</v>
       </c>
       <c r="C11" s="2">
-        <v>2.171</v>
+        <v>4.579</v>
       </c>
       <c r="D11" s="2">
-        <v>116.809242990561</v>
+        <v>120.257087462487</v>
       </c>
       <c r="E11" s="2">
-        <v>3.285</v>
+        <v>3.923</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1341,13 +1580,13 @@
         <v>26</v>
       </c>
       <c r="C12" s="2">
-        <v>2.945</v>
+        <v>3.998</v>
       </c>
       <c r="D12" s="2">
-        <v>115.268450034347</v>
+        <v>120.878252503199</v>
       </c>
       <c r="E12" s="2">
-        <v>2.984</v>
+        <v>3.556</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1358,13 +1597,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="2">
-        <v>2.999</v>
+        <v>2.698</v>
       </c>
       <c r="D13" s="2">
-        <v>113.365042963786</v>
+        <v>123.766078155408</v>
       </c>
       <c r="E13" s="2">
-        <v>2.627</v>
+        <v>3.299</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1375,13 +1614,13 @@
         <v>30</v>
       </c>
       <c r="C14" s="2">
-        <v>2.297</v>
+        <v>4.993</v>
       </c>
       <c r="D14" s="2">
-        <v>118.597040134681</v>
+        <v>120.738938632308</v>
       </c>
       <c r="E14" s="2">
-        <v>2.814</v>
+        <v>3.94</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1392,13 +1631,13 @@
         <v>32</v>
       </c>
       <c r="C15" s="2">
-        <v>4.189</v>
+        <v>4.53</v>
       </c>
       <c r="D15" s="2">
-        <v>120.128347245463</v>
+        <v>125.226937083884</v>
       </c>
       <c r="E15" s="2">
-        <v>3.959</v>
+        <v>3.622</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1409,13 +1648,13 @@
         <v>34</v>
       </c>
       <c r="C16" s="2">
-        <v>3.999</v>
+        <v>2.485</v>
       </c>
       <c r="D16" s="2">
-        <v>115.893419321157</v>
+        <v>129.202324904969</v>
       </c>
       <c r="E16" s="2">
-        <v>4.833</v>
+        <v>4.058</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1426,13 +1665,13 @@
         <v>36</v>
       </c>
       <c r="C17" s="2">
-        <v>1.499</v>
+        <v>3.017</v>
       </c>
       <c r="D17" s="2">
-        <v>115.950871731347</v>
+        <v>113.60833723178</v>
       </c>
       <c r="E17" s="2">
-        <v>3</v>
+        <v>2.641</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1443,254 +1682,694 @@
         <v>38</v>
       </c>
       <c r="C18" s="2">
-        <v>4.993</v>
+        <v>3.586</v>
       </c>
       <c r="D18" s="2">
-        <v>120.764775268163</v>
+        <v>122.692594631198</v>
       </c>
       <c r="E18" s="2">
-        <v>3.937</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
+        <v>3.507</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2.862</v>
+      </c>
+      <c r="D19" s="2">
+        <v>118.597937297662</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2.071</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3.912</v>
+      </c>
+      <c r="D20" s="2">
+        <v>123.168875600812</v>
+      </c>
+      <c r="E20" s="2">
+        <v>3.545</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3.781</v>
+      </c>
+      <c r="D21" s="2">
+        <v>121.257042304533</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4.444</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3.746</v>
+      </c>
+      <c r="D22" s="2">
+        <v>123.154857091523</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1.613</v>
+      </c>
+      <c r="D23" s="2">
+        <v>123.349385325636</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3.167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3.797</v>
+      </c>
+      <c r="D24" s="2">
+        <v>117.28717046366</v>
+      </c>
+      <c r="E24" s="2">
+        <v>4.115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2.217</v>
+      </c>
+      <c r="D25" s="2">
+        <v>119.204638033212</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2.992</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="2">
+        <v>4.596</v>
+      </c>
+      <c r="D26" s="2">
+        <v>120.76992039104</v>
+      </c>
+      <c r="E26" s="2">
+        <v>4.255</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="2">
+        <v>3.199</v>
+      </c>
+      <c r="D27" s="2">
+        <v>115.136965748452</v>
+      </c>
+      <c r="E27" s="2">
+        <v>3.575</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2.188</v>
+      </c>
+      <c r="D28" s="2">
+        <v>120.408407476382</v>
+      </c>
+      <c r="E28" s="2">
+        <v>3.682</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2.997</v>
+      </c>
+      <c r="D29" s="2">
+        <v>120.323647330667</v>
+      </c>
+      <c r="E29" s="2">
+        <v>3.559</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="2">
+        <v>4.61</v>
+      </c>
+      <c r="D30" s="2">
+        <v>115.576416237313</v>
+      </c>
+      <c r="E30" s="2">
+        <v>2.301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="2">
+        <v>4.189</v>
+      </c>
+      <c r="D31" s="2">
+        <v>120.11166833188</v>
+      </c>
+      <c r="E31" s="2">
+        <v>3.962</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2.171</v>
+      </c>
+      <c r="D32" s="2">
+        <v>116.813354720822</v>
+      </c>
+      <c r="E32" s="2">
+        <v>3.288</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2.496</v>
+      </c>
+      <c r="D33" s="2">
+        <v>123.617234201405</v>
+      </c>
+      <c r="E33" s="2">
+        <v>3.562</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2.61</v>
+      </c>
+      <c r="D34" s="2">
+        <v>113.356950390549</v>
+      </c>
+      <c r="E34" s="2">
+        <v>2.296</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2.999</v>
+      </c>
+      <c r="D35" s="2">
+        <v>113.351895282347</v>
+      </c>
+      <c r="E35" s="2">
+        <v>2.63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="2">
+        <v>2.982</v>
+      </c>
+      <c r="D36" s="2">
+        <v>123.378973808609</v>
+      </c>
+      <c r="E36" s="2">
+        <v>3.584</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="2">
+        <v>4.743</v>
+      </c>
+      <c r="D37" s="2">
+        <v>121.075347670685</v>
+      </c>
+      <c r="E37" s="2">
+        <v>3.504</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2.089</v>
+      </c>
+      <c r="D38" s="2">
+        <v>115.284491972009</v>
+      </c>
+      <c r="E38" s="2">
+        <v>3.252</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="2">
+        <v>3.011</v>
+      </c>
+      <c r="D39" s="2">
+        <v>120.465940931899</v>
+      </c>
+      <c r="E39" s="2">
+        <v>3.962</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2.441</v>
+      </c>
+      <c r="D40" s="2">
+        <v>121.305301566076</v>
+      </c>
+      <c r="E40" s="2">
+        <v>4.027</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="2">
+        <v>4.585</v>
+      </c>
+      <c r="D41" s="2">
+        <v>111.331037868457</v>
+      </c>
+      <c r="E41" s="2">
+        <v>2.258</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="2">
+        <v>3.999</v>
+      </c>
+      <c r="D42" s="2">
+        <v>115.840284097086</v>
+      </c>
+      <c r="E42" s="2">
+        <v>4.836</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="2">
+        <v>2.598</v>
+      </c>
+      <c r="D43" s="2">
+        <v>117.247189959741</v>
+      </c>
+      <c r="E43" s="2">
+        <v>3.548</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2.297</v>
+      </c>
+      <c r="D44" s="2">
+        <v>118.612344251333</v>
+      </c>
+      <c r="E44" s="2">
+        <v>2.816</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2.249</v>
+      </c>
+      <c r="D45" s="2">
+        <v>116.985983271414</v>
+      </c>
+      <c r="E45" s="2">
+        <v>3.162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="2">
+        <v>3.062</v>
+      </c>
+      <c r="D46" s="2">
+        <v>119.983504396819</v>
+      </c>
+      <c r="E46" s="2">
+        <v>3.978</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="2">
+        <v>3.79</v>
+      </c>
+      <c r="D47" s="2">
+        <v>112.278719129324</v>
+      </c>
+      <c r="E47" s="2">
+        <v>3.279</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="2">
+        <v>2.945</v>
+      </c>
+      <c r="D48" s="2">
+        <v>115.263164994523</v>
+      </c>
+      <c r="E48" s="2">
+        <v>2.986</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1.721</v>
+      </c>
+      <c r="D49" s="2">
+        <v>118.97567026139</v>
+      </c>
+      <c r="E49" s="2">
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1.499</v>
+      </c>
+      <c r="D50" s="2">
+        <v>117.128404476621</v>
+      </c>
+      <c r="E50" s="2">
+        <v>3.005</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51" s="2">
+        <v>3.755</v>
+      </c>
+      <c r="D51" s="2">
+        <v>116.733055809288</v>
+      </c>
+      <c r="E51" s="2">
+        <v>4.871</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="2">
+        <v>4.585</v>
+      </c>
+      <c r="D52" s="2">
+        <v>114.236014406613</v>
+      </c>
+      <c r="E52" s="2">
+        <v>3.162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="2">
+        <v>3.099</v>
+      </c>
+      <c r="D53" s="2">
+        <v>113.241175324706</v>
+      </c>
+      <c r="E53" s="2">
+        <v>2.997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="2">
+        <v>2.294</v>
+      </c>
+      <c r="D54" s="2">
+        <v>115.528221758498</v>
+      </c>
+      <c r="E54" s="2">
+        <v>2.51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" s="2">
+        <v>2.137</v>
+      </c>
+      <c r="D55" s="2">
+        <v>113.213803398441</v>
+      </c>
+      <c r="E55" s="2">
+        <v>2.795</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="2">
+        <v>2.798</v>
+      </c>
+      <c r="D56" s="2">
+        <v>114.177756428363</v>
+      </c>
+      <c r="E56" s="2">
+        <v>3.197</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="2">
+        <v>2.685</v>
+      </c>
+      <c r="D57" s="2">
+        <v>112.426151719058</v>
+      </c>
+      <c r="E57" s="2">
+        <v>2.564</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="2">
+        <v>4.159</v>
+      </c>
+      <c r="D58" s="2">
+        <v>112.415586065643</v>
+      </c>
+      <c r="E58" s="2">
+        <v>2.605</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>